<commit_message>
Start of Tonnage data insert
</commit_message>
<xml_diff>
--- a/Spreadsheet/TonnageData/2019-03-27 Tonnage End of the Year Crosstab 2018.xlsx
+++ b/Spreadsheet/TonnageData/2019-03-27 Tonnage End of the Year Crosstab 2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\TonnageData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8DBE544-346A-454E-AD7E-8F5B30EEE7D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD400D67-BF9A-4A08-A706-8506AB506F0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3480,7 +3480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="U68" sqref="U68"/>
@@ -3494,12 +3494,12 @@
     <col min="4" max="4" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
     <col min="14" max="14" width="15" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="13.42578125" style="8" bestFit="1" customWidth="1"/>

</xml_diff>